<commit_message>
added condition to appendMatches, no 0 amts
</commit_message>
<xml_diff>
--- a/account_recs.xlsx
+++ b/account_recs.xlsx
@@ -1,17 +1,18 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="Calc"/>
-  <workbookPr backupFile="false" showObjects="all" date1904="false"/>
+  <workbookPr showObjects="all"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView activeTab="1" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="500" windowHeight="8192" windowWidth="16384" xWindow="0" yWindow="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
-    <sheet name="megan" sheetId="2" state="hidden" r:id="rId3"/>
+    <sheet xmlns:relationships="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" relationships:id="rId2" state="visible"/>
+    <sheet xmlns:relationships="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="megan" sheetId="2" relationships:id="rId3" state="hidden"/>
+    <sheet xmlns:relationships="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="cats" sheetId="3" relationships:id="rId5"/>
   </sheets>
-  <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
+  <calcPr iterateCount="100" iterateDelta="0.001" refMode="A1"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="CalcA1"/>
@@ -139,14 +140,20 @@
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill patternType="none"/>
+      <patternFill patternType="none">
+        <fgColor/>
+        <bgColor/>
+      </patternFill>
     </fill>
     <fill>
-      <patternFill patternType="gray125"/>
+      <patternFill patternType="gray125">
+        <fgColor/>
+        <bgColor/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
-    <border diagonalUp="false" diagonalDown="false">
+    <border>
       <left/>
       <right/>
       <top/>
@@ -155,71 +162,71 @@
     </border>
   </borders>
   <cellStyleXfs count="20">
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf applyAlignment="true" applyBorder="true" applyFill="false" applyFont="true" applyNumberFormat="false" applyProtection="true" borderId="0" fillId="0" fontId="0" numFmtId="164">
+      <alignment horizontal="general" vertical="bottom"/>
+      <protection hidden="false" locked="true"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf applyAlignment="false" applyBorder="false" applyFill="false" applyFont="true" applyNumberFormat="false" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="0"/>
+    <xf applyAlignment="false" applyBorder="false" applyFill="false" applyFont="true" applyNumberFormat="false" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="0"/>
+    <xf applyAlignment="false" applyBorder="false" applyFill="false" applyFont="true" applyNumberFormat="false" applyProtection="false" borderId="0" fillId="0" fontId="2" numFmtId="0"/>
+    <xf applyAlignment="false" applyBorder="false" applyFill="false" applyFont="true" applyNumberFormat="false" applyProtection="false" borderId="0" fillId="0" fontId="2" numFmtId="0"/>
+    <xf applyAlignment="false" applyBorder="false" applyFill="false" applyFont="true" applyNumberFormat="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf applyAlignment="false" applyBorder="false" applyFill="false" applyFont="true" applyNumberFormat="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf applyAlignment="false" applyBorder="false" applyFill="false" applyFont="true" applyNumberFormat="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf applyAlignment="false" applyBorder="false" applyFill="false" applyFont="true" applyNumberFormat="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf applyAlignment="false" applyBorder="false" applyFill="false" applyFont="true" applyNumberFormat="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf applyAlignment="false" applyBorder="false" applyFill="false" applyFont="true" applyNumberFormat="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf applyAlignment="false" applyBorder="false" applyFill="false" applyFont="true" applyNumberFormat="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf applyAlignment="false" applyBorder="false" applyFill="false" applyFont="true" applyNumberFormat="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf applyAlignment="false" applyBorder="false" applyFill="false" applyFont="true" applyNumberFormat="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf applyAlignment="false" applyBorder="false" applyFill="false" applyFont="true" applyNumberFormat="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf applyAlignment="false" applyBorder="false" applyFill="false" applyFont="true" applyNumberFormat="false" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="43"/>
+    <xf applyAlignment="false" applyBorder="false" applyFill="false" applyFont="true" applyNumberFormat="false" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="41"/>
+    <xf applyAlignment="false" applyBorder="false" applyFill="false" applyFont="true" applyNumberFormat="false" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="44"/>
+    <xf applyAlignment="false" applyBorder="false" applyFill="false" applyFont="true" applyNumberFormat="false" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="42"/>
+    <xf applyAlignment="false" applyBorder="false" applyFill="false" applyFont="true" applyNumberFormat="false" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="9"/>
   </cellStyleXfs>
   <cellXfs count="2">
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf applyAlignment="false" applyBorder="false" applyFill="false" applyFont="false" applyNumberFormat="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0">
+      <alignment horizontal="general" vertical="bottom"/>
+      <protection hidden="false" locked="true"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf applyAlignment="false" applyBorder="false" applyFill="false" applyFont="false" applyNumberFormat="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0">
+      <alignment horizontal="general" vertical="bottom"/>
+      <protection hidden="false" locked="true"/>
     </xf>
   </cellXfs>
   <cellStyles count="6">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Comma" xfId="15" builtinId="3"/>
-    <cellStyle name="Comma [0]" xfId="16" builtinId="6"/>
-    <cellStyle name="Currency" xfId="17" builtinId="4"/>
-    <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
-    <cellStyle name="Percent" xfId="19" builtinId="5"/>
+    <cellStyle builtinId="0" name="Normal" xfId="0"/>
+    <cellStyle builtinId="3" name="Comma" xfId="15"/>
+    <cellStyle builtinId="6" name="Comma [0]" xfId="16"/>
+    <cellStyle builtinId="4" name="Currency" xfId="17"/>
+    <cellStyle builtinId="7" name="Currency [0]" xfId="18"/>
+    <cellStyle builtinId="5" name="Percent" xfId="19"/>
   </cellStyles>
 </styleSheet>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
+<worksheet xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xr:uid="{00000000-0001-0000-0000-000000000000}" mc:Ignorable="x14ac xr xr2 xr3">
+  <sheetPr>
+    <pageSetUpPr/>
   </sheetPr>
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E35" activeCellId="0" sqref="E35"/>
+    <sheetView showGridLines="true" showRowColHeaders="true" showZeros="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection activeCell="E35" activeCellId="0" pane="topLeft" sqref="E35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="1" style="1" width="11.52"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="1" width="11.52"/>
   </cols>
   <sheetData/>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
+  <printOptions gridLinesSet="true"/>
+  <pageMargins bottom="1.05277777777778" footer="0.7875" header="0.7875" left="0.7875" right="0.7875" top="1.05277777777778"/>
+  <pageSetup cellComments="none" copies="1" firstPageNumber="1" fitToHeight="1" fitToWidth="1" horizontalDpi="300" orientation="portrait" pageOrder="downThenOver" paperSize="1" scale="100" useFirstPageNumber="true" verticalDpi="300"/>
+  <headerFooter>
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
@@ -227,182 +234,359 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
+<worksheet xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xr:uid="{00000000-0001-0000-0000-000000000000}" mc:Ignorable="x14ac xr xr2 xr3">
+  <sheetPr>
+    <pageSetUpPr/>
   </sheetPr>
   <dimension ref="A1:C14"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    <sheetView showGridLines="true" showRowColHeaders="true" showZeros="true" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection activeCell="A1" activeCellId="0" pane="topLeft" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="8.51"/>
+    <col collapsed="false" customWidth="true" hidden="false" max="1025" min="1" style="0" width="8.51"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="n">
+    <row ht="12.8" r="1">
+      <c r="A1" t="n">
         <v>150</v>
       </c>
-      <c r="B1" s="0" t="s">
+      <c r="B1" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="0" t="s">
+      <c r="C1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="n">
+    <row ht="12.8" r="2">
+      <c r="A2" t="n">
         <v>200</v>
       </c>
-      <c r="B2" s="0" t="s">
+      <c r="B2" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="0" t="s">
+      <c r="C2" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="n">
+    <row ht="12.8" r="3">
+      <c r="A3" t="n">
         <v>350</v>
       </c>
-      <c r="B3" s="0" t="s">
+      <c r="B3" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="0" t="s">
+      <c r="C3" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="n">
+    <row ht="12.8" r="4">
+      <c r="A4" t="n">
         <v>400</v>
       </c>
-      <c r="B4" s="0" t="s">
+      <c r="B4" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="0" t="s">
+      <c r="C4" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="n">
+    <row ht="12.8" r="5">
+      <c r="A5" t="n">
         <v>650</v>
       </c>
-      <c r="B5" s="0" t="s">
+      <c r="B5" t="s">
         <v>8</v>
       </c>
-      <c r="C5" s="0" t="s">
+      <c r="C5" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0" t="n">
+    <row ht="12.8" r="6">
+      <c r="A6" t="n">
         <v>700</v>
       </c>
-      <c r="B6" s="0" t="s">
+      <c r="B6" t="s">
         <v>10</v>
       </c>
-      <c r="C6" s="0" t="s">
+      <c r="C6" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="0" t="n">
+    <row ht="12.8" r="7">
+      <c r="A7" t="n">
         <v>750</v>
       </c>
-      <c r="B7" s="0" t="s">
+      <c r="B7" t="s">
         <v>12</v>
       </c>
-      <c r="C7" s="0" t="s">
+      <c r="C7" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="0" t="n">
+    <row ht="12.8" r="8">
+      <c r="A8" t="n">
         <v>800</v>
       </c>
-      <c r="B8" s="0" t="s">
+      <c r="B8" t="s">
         <v>14</v>
       </c>
-      <c r="C8" s="0" t="s">
+      <c r="C8" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="0" t="n">
+    <row ht="12.8" r="9">
+      <c r="A9" t="n">
         <v>950</v>
       </c>
-      <c r="B9" s="0" t="s">
+      <c r="B9" t="s">
         <v>16</v>
       </c>
-      <c r="C9" s="0" t="s">
+      <c r="C9" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="0" t="n">
+    <row ht="12.8" r="10">
+      <c r="A10" t="n">
         <v>1000</v>
       </c>
-      <c r="B10" s="0" t="s">
+      <c r="B10" t="s">
         <v>18</v>
       </c>
-      <c r="C10" s="0" t="s">
+      <c r="C10" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="0" t="n">
+    <row ht="12.8" r="11">
+      <c r="A11" t="n">
         <v>1050</v>
       </c>
-      <c r="B11" s="0" t="s">
+      <c r="B11" t="s">
         <v>20</v>
       </c>
-      <c r="C11" s="0" t="s">
+      <c r="C11" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="0" t="n">
+    <row ht="12.8" r="12">
+      <c r="A12" t="n">
         <v>1100</v>
       </c>
-      <c r="B12" s="0" t="s">
+      <c r="B12" t="s">
         <v>22</v>
       </c>
-      <c r="C12" s="0" t="s">
+      <c r="C12" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="0" t="n">
+    <row ht="12.8" r="13">
+      <c r="A13" t="n">
         <v>1250</v>
       </c>
-      <c r="B13" s="0" t="s">
+      <c r="B13" t="s">
         <v>24</v>
       </c>
-      <c r="C13" s="0" t="s">
+      <c r="C13" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="0" t="n">
+    <row ht="12.8" r="14">
+      <c r="A14" t="n">
         <v>1300</v>
       </c>
-      <c r="B14" s="0" t="s">
+      <c r="B14" t="s">
         <v>26</v>
       </c>
-      <c r="C14" s="0" t="s">
+      <c r="C14" t="s">
         <v>27</v>
       </c>
     </row>
   </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
+  <printOptions gridLinesSet="true"/>
+  <pageMargins bottom="0.984027777777778" footer="0.511805555555555" header="0.511805555555555" left="0.747916666666667" right="0.747916666666667" top="0.984027777777778"/>
+  <pageSetup cellComments="none" copies="1" fitToHeight="1" fitToWidth="1" horizontalDpi="300" orientation="portrait" pageOrder="downThenOver" paperSize="1" scale="100" verticalDpi="300"/>
+  <headerFooter>
     <oddHeader/>
     <oddFooter/>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xr:uid="{00000000-0001-0000-0000-000000000000}" mc:Ignorable="x14ac xr xr2 xr3">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetData>
+    <row r="1"/>
+    <row r="2"/>
+    <row r="3">
+      <c r="A3">
+        <v>150</v>
+      </c>
+      <c r="B3" t="str">
+        <v>hgfd</v>
+      </c>
+      <c r="C3" t="str">
+        <v>43468</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4">
+        <v>200</v>
+      </c>
+      <c r="B4" t="str">
+        <v>jhgf</v>
+      </c>
+      <c r="C4" t="str">
+        <v>43469</v>
+      </c>
+    </row>
+    <row r="5"/>
+    <row r="6"/>
+    <row r="7">
+      <c r="A7">
+        <v>350</v>
+      </c>
+      <c r="B7" t="str">
+        <v>trew</v>
+      </c>
+      <c r="C7" t="str">
+        <v>43472</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8">
+        <v>400</v>
+      </c>
+      <c r="B8" t="str">
+        <v>ytre</v>
+      </c>
+      <c r="C8" t="str">
+        <v>43473</v>
+      </c>
+    </row>
+    <row r="9"/>
+    <row r="10"/>
+    <row r="11"/>
+    <row r="12"/>
+    <row r="13">
+      <c r="A13">
+        <v>650</v>
+      </c>
+      <c r="B13" t="str">
+        <v>zxcv</v>
+      </c>
+      <c r="C13" t="str">
+        <v>43478</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14">
+        <v>700</v>
+      </c>
+      <c r="B14" t="str">
+        <v>xcvb</v>
+      </c>
+      <c r="C14" t="str">
+        <v>43479</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15">
+        <v>750</v>
+      </c>
+      <c r="B15" t="str">
+        <v>cvbn</v>
+      </c>
+      <c r="C15" t="str">
+        <v>43480</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16">
+        <v>800</v>
+      </c>
+      <c r="B16" t="str">
+        <v>vbnm</v>
+      </c>
+      <c r="C16" t="str">
+        <v>43481</v>
+      </c>
+    </row>
+    <row r="17"/>
+    <row r="18"/>
+    <row r="19">
+      <c r="A19">
+        <v>950</v>
+      </c>
+      <c r="B19" t="str">
+        <v>dfgh</v>
+      </c>
+      <c r="C19" t="str">
+        <v>43484</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20">
+        <v>1000</v>
+      </c>
+      <c r="B20" t="str">
+        <v>fghj</v>
+      </c>
+      <c r="C20" t="str">
+        <v>43485</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21">
+        <v>1050</v>
+      </c>
+      <c r="B21" t="str">
+        <v>ghjk</v>
+      </c>
+      <c r="C21" t="str">
+        <v>43486</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22">
+        <v>1100</v>
+      </c>
+      <c r="B22" t="str">
+        <v>hgjkl</v>
+      </c>
+      <c r="C22" t="str">
+        <v>43487</v>
+      </c>
+    </row>
+    <row r="23"/>
+    <row r="24"/>
+    <row r="25">
+      <c r="A25">
+        <v>1250</v>
+      </c>
+      <c r="B25" t="str">
+        <v>erty</v>
+      </c>
+      <c r="C25" t="str">
+        <v>43490</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26">
+        <v>1300</v>
+      </c>
+      <c r="B26" t="str">
+        <v>rtyu</v>
+      </c>
+      <c r="C26" t="str">
+        <v>43491</v>
+      </c>
+    </row>
+  </sheetData>
+</worksheet>
 </file>
</xml_diff>